<commit_message>
Updated site enablement playbook for voice download file.
</commit_message>
<xml_diff>
--- a/Teams/downloads/site-enablement-playbook-for-voice-(playbook).xlsx
+++ b/Teams/downloads/site-enablement-playbook-for-voice-(playbook).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19120"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19316"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0DEC13-93DF-4779-B909-82664FBFA025}" xr6:coauthVersionLast="30" xr6:coauthVersionMax="30" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604DDB3E-DB3C-44DE-8B4E-0F183B504650}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" tabRatio="692" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12816" tabRatio="692" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="3" r:id="rId1"/>
@@ -77,19 +77,19 @@
     <definedName name="_3.2.5">'[1]3-User Enablement'!#REF!</definedName>
     <definedName name="_3.2.9">'[1]3-User Enablement'!#REF!</definedName>
     <definedName name="_4.1.1">'4-Endpoints'!$B$5</definedName>
-    <definedName name="_4.1.2">'4-Endpoints'!$B$6</definedName>
+    <definedName name="_4.1.2">'4-Endpoints'!$B$7</definedName>
     <definedName name="_4.1.3">'[1]4-Endpoints'!#REF!</definedName>
-    <definedName name="_4.2.1">'4-Endpoints'!$B$9</definedName>
+    <definedName name="_4.2.1">'4-Endpoints'!$B$10</definedName>
     <definedName name="_4.2.10">'[1]4-Endpoints'!#REF!</definedName>
     <definedName name="_4.2.11">'[1]4-Endpoints'!#REF!</definedName>
     <definedName name="_4.2.12">'[1]4-Endpoints'!#REF!</definedName>
-    <definedName name="_4.2.2">'4-Endpoints'!$B$10</definedName>
-    <definedName name="_4.2.3">'4-Endpoints'!$B$11</definedName>
-    <definedName name="_4.2.4">'4-Endpoints'!$B$12</definedName>
-    <definedName name="_4.2.5">'4-Endpoints'!$B$13</definedName>
+    <definedName name="_4.2.2">'4-Endpoints'!$B$11</definedName>
+    <definedName name="_4.2.3">'4-Endpoints'!$B$12</definedName>
+    <definedName name="_4.2.4">'4-Endpoints'!$B$13</definedName>
+    <definedName name="_4.2.5">'4-Endpoints'!$B$14</definedName>
     <definedName name="_4.2.6" localSheetId="1">'[1]4-Endpoints'!#REF!</definedName>
-    <definedName name="_4.2.6">'4-Endpoints'!$B$14</definedName>
-    <definedName name="_4.2.7">'4-Endpoints'!$B$15</definedName>
+    <definedName name="_4.2.6">'4-Endpoints'!$B$15</definedName>
+    <definedName name="_4.2.7">'4-Endpoints'!$B$16</definedName>
     <definedName name="_4.2.8">'[1]4-Endpoints'!#REF!</definedName>
     <definedName name="_4.3.1">'[1]4-Endpoints'!#REF!</definedName>
     <definedName name="_4.3.10">'[1]4-Endpoints'!#REF!</definedName>
@@ -961,9 +961,6 @@
     <t>Operations Guide</t>
   </si>
   <si>
-    <t>Assessing Teams Usage</t>
-  </si>
-  <si>
     <t>Capture detailed information that will assist you in planning the rollout of Teams voice workloads to the site</t>
   </si>
   <si>
@@ -1292,35 +1289,6 @@
   </si>
   <si>
     <t>4.1.1 - Deploy the Teams client on user workstations, laptops, and mobile devices</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Teams has clients available for web, desktop (Windows and Mac), and mobile (Android, iOS, and Windows Phone). These clients all require an active internet connection.
-Desktop clients can be downloaded and installed by users directly from https://teams.microsoft.com/downloads, or IT admins can use existing software management solutions to distribute installation files to client machines.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Distribution of the Teams client via software management solutions is only available for the initial installation of Teams clients, and not for future updates.
-Teams clients are updated automatically by the Teams service with no IT administrator intervention required.</t>
-    </r>
   </si>
   <si>
     <t>Notify users about the Office 365 self-service portal for installing software to personal devices</t>
@@ -1619,6 +1587,39 @@
   <si>
     <t>Set up Communications Credits for your tenant to provide toll-free access for your organization’s conference bridge phone numbers, or give conference organizers the ability to dial out to international meeting participants.
 Validate that Communications Credits have been added to your tenant to support the functionalities described above.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Teams has clients available for web, desktop (Windows and Mac), and mobile (Android, iOS, and Windows Phone). These clients all require an active internet connection.
+Desktop clients can be downloaded and installed by users directly from https://teams.microsoft.com/downloads, or IT admins can use existing software management solutions to distribute installation files to client machines.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Distribution of the Teams client via software management solutions is only available for the initial installation of Teams clients, and not for future updates.
+Teams clients are updated automatically by the Teams service with no IT administrator intervention required.
+Teams also has MSI package available to IT Administrators for deployment via ITPro tools.</t>
+    </r>
+  </si>
+  <si>
+    <t>Install Microsoft Teams using MSI</t>
   </si>
 </sst>
 </file>
@@ -2294,7 +2295,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="432">
+  <cellXfs count="440">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3308,14 +3309,89 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="11" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="11" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3377,75 +3453,6 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3458,33 +3465,21 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="37" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3500,6 +3495,18 @@
     <xf numFmtId="49" fontId="37" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3561,6 +3568,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6229,19 +6254,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="Q12:W20"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="23:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="23:23" x14ac:dyDescent="0.3">
       <c r="W12"/>
     </row>
-    <row r="20" spans="17:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="17:17" x14ac:dyDescent="0.3">
       <c r="Q20"/>
     </row>
   </sheetData>
@@ -6257,27 +6280,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="101" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="100" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="98" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="99" t="s">
         <v>40</v>
       </c>
@@ -6296,7 +6319,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="298"/>
     <col min="2" max="2" width="61" style="298" customWidth="1"/>
@@ -6304,7 +6327,7 @@
     <col min="4" max="16384" width="9" style="298"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="308" t="s">
         <v>116</v>
       </c>
@@ -6315,7 +6338,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="299" t="s">
         <v>139</v>
       </c>
@@ -6326,28 +6349,28 @@
         <v>43126</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="301"/>
       <c r="B3" s="302"/>
       <c r="C3" s="300"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="303"/>
       <c r="B4" s="304"/>
       <c r="C4" s="305"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="303"/>
       <c r="B5" s="306"/>
       <c r="C5" s="305"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="307"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="307"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="307"/>
     </row>
   </sheetData>
@@ -6368,120 +6391,120 @@
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="17" customWidth="1"/>
-    <col min="2" max="2" width="28.36328125" style="17" customWidth="1"/>
-    <col min="3" max="12" width="18.54296875" style="17" customWidth="1"/>
-    <col min="13" max="13" width="25.90625" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="18.54296875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="17" customWidth="1"/>
+    <col min="3" max="12" width="18.5546875" style="17" customWidth="1"/>
+    <col min="13" max="13" width="25.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="18.5546875" style="17" customWidth="1"/>
     <col min="20" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:19" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:19" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="114" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="114" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="370" t="s">
+      <c r="D2" s="363" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="370"/>
-    </row>
-    <row r="3" spans="2:19" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E2" s="363"/>
+    </row>
+    <row r="3" spans="2:19" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="113" t="s">
         <v>114</v>
       </c>
       <c r="C3" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="371">
+      <c r="D3" s="364">
         <v>43179</v>
       </c>
-      <c r="E3" s="371"/>
-    </row>
-    <row r="4" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="2:19" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="375" t="str">
+      <c r="E3" s="364"/>
+    </row>
+    <row r="4" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:19" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="368" t="str">
         <f>"Site rollout schedule for site: " &amp; B3 &amp; " - " &amp; C3</f>
         <v>Site rollout schedule for site: {SiteName} - {SiteCode}</v>
       </c>
-      <c r="C5" s="376"/>
-      <c r="D5" s="376"/>
-      <c r="E5" s="376"/>
-      <c r="F5" s="376"/>
-      <c r="G5" s="376"/>
-      <c r="H5" s="376"/>
-      <c r="I5" s="376"/>
-      <c r="J5" s="376"/>
-      <c r="K5" s="376"/>
-      <c r="L5" s="376"/>
-      <c r="M5" s="376"/>
-      <c r="N5" s="376"/>
-      <c r="O5" s="376"/>
-      <c r="P5" s="376"/>
-      <c r="Q5" s="376"/>
-      <c r="R5" s="376"/>
-      <c r="S5" s="377"/>
-    </row>
-    <row r="6" spans="2:19" s="19" customFormat="1" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="379" t="s">
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
+      <c r="G5" s="369"/>
+      <c r="H5" s="369"/>
+      <c r="I5" s="369"/>
+      <c r="J5" s="369"/>
+      <c r="K5" s="369"/>
+      <c r="L5" s="369"/>
+      <c r="M5" s="369"/>
+      <c r="N5" s="369"/>
+      <c r="O5" s="369"/>
+      <c r="P5" s="369"/>
+      <c r="Q5" s="369"/>
+      <c r="R5" s="369"/>
+      <c r="S5" s="370"/>
+    </row>
+    <row r="6" spans="2:19" s="19" customFormat="1" ht="26.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="372" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" s="372"/>
+      <c r="D6" s="372"/>
+      <c r="E6" s="372"/>
+      <c r="F6" s="372"/>
+      <c r="G6" s="372"/>
+      <c r="H6" s="372"/>
+      <c r="I6" s="372"/>
+      <c r="J6" s="372"/>
+      <c r="K6" s="372"/>
+      <c r="L6" s="372"/>
+      <c r="M6" s="316" t="s">
+        <v>327</v>
+      </c>
+      <c r="N6" s="371" t="s">
         <v>328</v>
       </c>
-      <c r="C6" s="379"/>
-      <c r="D6" s="379"/>
-      <c r="E6" s="379"/>
-      <c r="F6" s="379"/>
-      <c r="G6" s="379"/>
-      <c r="H6" s="379"/>
-      <c r="I6" s="379"/>
-      <c r="J6" s="379"/>
-      <c r="K6" s="379"/>
-      <c r="L6" s="379"/>
-      <c r="M6" s="316" t="s">
+      <c r="O6" s="371"/>
+      <c r="P6" s="371"/>
+      <c r="Q6" s="371"/>
+      <c r="R6" s="371"/>
+      <c r="S6" s="371"/>
+    </row>
+    <row r="7" spans="2:19" s="6" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="317" t="s">
         <v>329</v>
       </c>
-      <c r="N6" s="378" t="s">
+      <c r="C7" s="365" t="s">
         <v>330</v>
       </c>
-      <c r="O6" s="378"/>
-      <c r="P6" s="378"/>
-      <c r="Q6" s="378"/>
-      <c r="R6" s="378"/>
-      <c r="S6" s="378"/>
-    </row>
-    <row r="7" spans="2:19" s="6" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="317" t="s">
+      <c r="D7" s="366"/>
+      <c r="E7" s="366"/>
+      <c r="F7" s="366"/>
+      <c r="G7" s="366"/>
+      <c r="H7" s="366"/>
+      <c r="I7" s="366"/>
+      <c r="J7" s="366"/>
+      <c r="K7" s="366"/>
+      <c r="L7" s="367"/>
+      <c r="M7" s="373" t="s">
+        <v>96</v>
+      </c>
+      <c r="N7" s="365" t="s">
         <v>331</v>
       </c>
-      <c r="C7" s="372" t="s">
-        <v>332</v>
-      </c>
-      <c r="D7" s="373"/>
-      <c r="E7" s="373"/>
-      <c r="F7" s="373"/>
-      <c r="G7" s="373"/>
-      <c r="H7" s="373"/>
-      <c r="I7" s="373"/>
-      <c r="J7" s="373"/>
-      <c r="K7" s="373"/>
-      <c r="L7" s="374"/>
-      <c r="M7" s="380" t="s">
-        <v>96</v>
-      </c>
-      <c r="N7" s="372" t="s">
-        <v>333</v>
-      </c>
-      <c r="O7" s="373"/>
-      <c r="P7" s="373"/>
-      <c r="Q7" s="373"/>
-      <c r="R7" s="373"/>
-      <c r="S7" s="374"/>
-    </row>
-    <row r="8" spans="2:19" s="18" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O7" s="366"/>
+      <c r="P7" s="366"/>
+      <c r="Q7" s="366"/>
+      <c r="R7" s="366"/>
+      <c r="S7" s="367"/>
+    </row>
+    <row r="8" spans="2:19" s="18" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="317" t="s">
         <v>31</v>
       </c>
@@ -6515,7 +6538,7 @@
       <c r="L8" s="309" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="381"/>
+      <c r="M8" s="374"/>
       <c r="N8" s="309" t="s">
         <v>32</v>
       </c>
@@ -6535,7 +6558,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:19" s="18" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:19" s="18" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="317" t="s">
         <v>101</v>
       </c>
@@ -6608,9 +6631,9 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="10" spans="2:19" s="61" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:19" s="61" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="318" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C10" s="60">
         <f>MAX('1-Playbook Preparation'!C5,'1-Playbook Preparation'!C9)</f>
@@ -6621,35 +6644,35 @@
         <v>1</v>
       </c>
       <c r="E10" s="60">
-        <f>MAX('1-Playbook Preparation'!C6,'2-Site Voice Readiness'!C5,'2-Site Voice Readiness'!C6,'3-User Enablement'!C6,'4-Endpoints'!C9,'4-Endpoints'!C10)</f>
+        <f>MAX('1-Playbook Preparation'!C6,'2-Site Voice Readiness'!C5,'2-Site Voice Readiness'!C6,'3-User Enablement'!C6,'4-Endpoints'!C10,'4-Endpoints'!C11)</f>
         <v>1</v>
       </c>
       <c r="F10" s="60">
-        <f>MAX('1-Playbook Preparation'!C10,'1-Playbook Preparation'!C11,'2-Site Voice Readiness'!C33,'2-Site Voice Readiness'!C7:C9,'2-Site Voice Readiness'!C15,'4-Endpoints'!C10,'4-Endpoints'!C13,'6-Adoption'!C11)</f>
+        <f>MAX('1-Playbook Preparation'!C10,'1-Playbook Preparation'!C11,'2-Site Voice Readiness'!C33,'2-Site Voice Readiness'!C7:C9,'2-Site Voice Readiness'!C15,'4-Endpoints'!C11,'4-Endpoints'!C14,'6-Adoption'!C11)</f>
         <v>1</v>
       </c>
       <c r="G10" s="93">
-        <f>MAX('2-Site Voice Readiness'!C16,'2-Site Voice Readiness'!C17:C19,'2-Site Voice Readiness'!C22,'2-Site Voice Readiness'!C10:C11,'4-Endpoints'!C10,'4-Endpoints'!C11,'6-Adoption'!C12,'6-Adoption'!C7,'5-Usage &amp; Quality'!C7)</f>
+        <f>MAX('2-Site Voice Readiness'!C16,'2-Site Voice Readiness'!C17:C19,'2-Site Voice Readiness'!C22,'2-Site Voice Readiness'!C10:C11,'4-Endpoints'!C11,'4-Endpoints'!C12,'6-Adoption'!C12,'6-Adoption'!C7,'5-Usage &amp; Quality'!C7)</f>
         <v>1</v>
       </c>
       <c r="H10" s="93">
-        <f>MAX('2-Site Voice Readiness'!C12,'4-Endpoints'!C10,'4-Endpoints'!C12,'6-Adoption'!C5,'6-Adoption'!C13,'5-Usage &amp; Quality'!C7)</f>
+        <f>MAX('2-Site Voice Readiness'!C12,'4-Endpoints'!C11,'4-Endpoints'!C13,'6-Adoption'!C5,'6-Adoption'!C13,'5-Usage &amp; Quality'!C7)</f>
         <v>1</v>
       </c>
       <c r="I10" s="93">
-        <f>MAX('3-User Enablement'!C8:C10,'3-User Enablement'!C11,'4-Endpoints'!C5,'4-Endpoints'!C6,'5-Usage &amp; Quality'!C7)</f>
+        <f>MAX('3-User Enablement'!C8:C10,'3-User Enablement'!C11,'4-Endpoints'!C5,'4-Endpoints'!C7,'5-Usage &amp; Quality'!C7)</f>
         <v>1</v>
       </c>
       <c r="J10" s="93">
-        <f>MAX('4-Endpoints'!C14,'4-Endpoints'!C5,'6-Adoption'!C23,'6-Adoption'!C17,'6-Adoption'!C27,'6-Adoption'!C8,'5-Usage &amp; Quality'!C7)</f>
+        <f>MAX('4-Endpoints'!C15,'4-Endpoints'!C5,'6-Adoption'!C23,'6-Adoption'!C17,'6-Adoption'!C27,'6-Adoption'!C8,'5-Usage &amp; Quality'!C7)</f>
         <v>1</v>
       </c>
       <c r="K10" s="93">
-        <f>MAX('2-Site Voice Readiness'!C23,'2-Site Voice Readiness'!C24:C26,'2-Site Voice Readiness'!C27,'2-Site Voice Readiness'!C30,'4-Endpoints'!C15,'4-Endpoints'!C5,'6-Adoption'!C18,'6-Adoption'!C6,'6-Adoption'!C27,'5-Usage &amp; Quality'!C7)</f>
+        <f>MAX('2-Site Voice Readiness'!C23,'2-Site Voice Readiness'!C24:C26,'2-Site Voice Readiness'!C27,'2-Site Voice Readiness'!C30,'4-Endpoints'!C16,'4-Endpoints'!C5,'6-Adoption'!C18,'6-Adoption'!C6,'6-Adoption'!C27,'5-Usage &amp; Quality'!C7)</f>
         <v>1</v>
       </c>
       <c r="L10" s="93">
-        <f>MAX('2-Site Voice Readiness'!C29,'3-User Enablement'!C12,'3-User Enablement'!C13,'3-User Enablement'!C14,'3-User Enablement'!C15,'3-User Enablement'!C16,'3-User Enablement'!C17,'4-Endpoints'!C15,'5-Usage &amp; Quality'!C7,'6-Adoption'!C20)</f>
+        <f>MAX('2-Site Voice Readiness'!C29,'3-User Enablement'!C12,'3-User Enablement'!C13,'3-User Enablement'!C14,'3-User Enablement'!C15,'3-User Enablement'!C16,'3-User Enablement'!C17,'4-Endpoints'!C16,'5-Usage &amp; Quality'!C7,'6-Adoption'!C20)</f>
         <v>1</v>
       </c>
       <c r="M10" s="93">
@@ -6681,8 +6704,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:19" s="61" customFormat="1" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="382" t="s">
+    <row r="11" spans="2:19" s="61" customFormat="1" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="352" t="s">
         <v>199</v>
       </c>
       <c r="C11" s="94" t="s">
@@ -6691,10 +6714,10 @@
       <c r="D11" s="94" t="s">
         <v>205</v>
       </c>
-      <c r="E11" s="384" t="s">
-        <v>337</v>
-      </c>
-      <c r="F11" s="386"/>
+      <c r="E11" s="354" t="s">
+        <v>335</v>
+      </c>
+      <c r="F11" s="356"/>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
       <c r="I11" s="95"/>
@@ -6709,15 +6732,15 @@
       <c r="R11" s="95"/>
       <c r="S11" s="95"/>
     </row>
-    <row r="12" spans="2:19" s="61" customFormat="1" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="383"/>
-      <c r="C12" s="384" t="s">
+    <row r="12" spans="2:19" s="61" customFormat="1" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="353"/>
+      <c r="C12" s="354" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="385"/>
+      <c r="D12" s="355"/>
       <c r="E12" s="96"/>
       <c r="F12" s="97" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G12" s="289"/>
       <c r="H12" s="289"/>
@@ -6733,8 +6756,8 @@
       <c r="R12" s="289"/>
       <c r="S12" s="289"/>
     </row>
-    <row r="13" spans="2:19" s="9" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="387" t="s">
+    <row r="13" spans="2:19" s="9" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="357" t="s">
         <v>200</v>
       </c>
       <c r="C13" s="130"/>
@@ -6743,7 +6766,7 @@
         <v>91</v>
       </c>
       <c r="F13" s="121" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G13" s="122" t="s">
         <v>210</v>
@@ -6767,15 +6790,15 @@
       <c r="R13" s="131"/>
       <c r="S13" s="131"/>
     </row>
-    <row r="14" spans="2:19" s="9" customFormat="1" ht="91.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="388"/>
+    <row r="14" spans="2:19" s="9" customFormat="1" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="358"/>
       <c r="C14" s="132"/>
       <c r="D14" s="132"/>
       <c r="E14" s="122" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F14" s="122" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G14" s="122" t="s">
         <v>211</v>
@@ -6795,16 +6818,16 @@
       <c r="R14" s="131"/>
       <c r="S14" s="131"/>
     </row>
-    <row r="15" spans="2:19" s="9" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="388"/>
+    <row r="15" spans="2:19" s="9" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="358"/>
       <c r="C15" s="132"/>
       <c r="D15" s="132"/>
       <c r="E15" s="131"/>
       <c r="F15" s="122" t="s">
+        <v>342</v>
+      </c>
+      <c r="G15" s="122" t="s">
         <v>344</v>
-      </c>
-      <c r="G15" s="122" t="s">
-        <v>346</v>
       </c>
       <c r="H15" s="122"/>
       <c r="I15" s="131"/>
@@ -6821,8 +6844,8 @@
       <c r="R15" s="131"/>
       <c r="S15" s="131"/>
     </row>
-    <row r="16" spans="2:19" s="9" customFormat="1" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="389"/>
+    <row r="16" spans="2:19" s="9" customFormat="1" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="359"/>
       <c r="C16" s="132"/>
       <c r="D16" s="132"/>
       <c r="E16" s="133"/>
@@ -6845,27 +6868,27 @@
       <c r="R16" s="131"/>
       <c r="S16" s="131"/>
     </row>
-    <row r="17" spans="2:19" ht="89.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="390" t="s">
+    <row r="17" spans="2:19" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="360" t="s">
         <v>122</v>
       </c>
       <c r="C17" s="123"/>
       <c r="D17" s="123" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E17" s="127" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F17" s="124"/>
       <c r="G17" s="134"/>
       <c r="H17" s="123"/>
       <c r="I17" s="123" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J17" s="125"/>
       <c r="K17" s="134"/>
       <c r="L17" s="123" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M17" s="129"/>
       <c r="N17" s="134"/>
@@ -6875,8 +6898,8 @@
       <c r="R17" s="134"/>
       <c r="S17" s="134"/>
     </row>
-    <row r="18" spans="2:19" ht="39" x14ac:dyDescent="0.35">
-      <c r="B18" s="391"/>
+    <row r="18" spans="2:19" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B18" s="361"/>
       <c r="C18" s="135"/>
       <c r="D18" s="135"/>
       <c r="E18" s="127" t="s">
@@ -6891,7 +6914,7 @@
       <c r="J18" s="127"/>
       <c r="K18" s="136"/>
       <c r="L18" s="127" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="M18" s="137"/>
       <c r="N18" s="136"/>
@@ -6901,8 +6924,8 @@
       <c r="R18" s="136"/>
       <c r="S18" s="136"/>
     </row>
-    <row r="19" spans="2:19" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="391"/>
+    <row r="19" spans="2:19" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="361"/>
       <c r="C19" s="135"/>
       <c r="D19" s="135"/>
       <c r="E19" s="136"/>
@@ -6923,8 +6946,8 @@
       <c r="R19" s="136"/>
       <c r="S19" s="136"/>
     </row>
-    <row r="20" spans="2:19" ht="52.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="391"/>
+    <row r="20" spans="2:19" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="361"/>
       <c r="C20" s="135"/>
       <c r="D20" s="135"/>
       <c r="E20" s="136"/>
@@ -6935,7 +6958,7 @@
       <c r="J20" s="137"/>
       <c r="K20" s="136"/>
       <c r="L20" s="128" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M20" s="137"/>
       <c r="N20" s="136"/>
@@ -6945,8 +6968,8 @@
       <c r="R20" s="136"/>
       <c r="S20" s="136"/>
     </row>
-    <row r="21" spans="2:19" ht="52.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="391"/>
+    <row r="21" spans="2:19" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="361"/>
       <c r="C21" s="135"/>
       <c r="D21" s="135"/>
       <c r="E21" s="136"/>
@@ -6957,7 +6980,7 @@
       <c r="J21" s="137"/>
       <c r="K21" s="136"/>
       <c r="L21" s="128" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M21" s="137"/>
       <c r="N21" s="136"/>
@@ -6967,8 +6990,8 @@
       <c r="R21" s="136"/>
       <c r="S21" s="136"/>
     </row>
-    <row r="22" spans="2:19" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="392"/>
+    <row r="22" spans="2:19" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="362"/>
       <c r="C22" s="135"/>
       <c r="D22" s="135"/>
       <c r="E22" s="136"/>
@@ -6989,14 +7012,14 @@
       <c r="R22" s="136"/>
       <c r="S22" s="136"/>
     </row>
-    <row r="23" spans="2:19" ht="95.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="353" t="s">
+    <row r="23" spans="2:19" ht="95.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="378" t="s">
         <v>123</v>
       </c>
       <c r="C23" s="138"/>
       <c r="D23" s="120"/>
       <c r="E23" s="29" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F23" s="29" t="s">
         <v>93</v>
@@ -7008,48 +7031,48 @@
         <v>94</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>335</v>
-      </c>
-      <c r="K23" s="350" t="s">
-        <v>351</v>
-      </c>
-      <c r="L23" s="352"/>
-      <c r="M23" s="350"/>
-      <c r="N23" s="351"/>
-      <c r="O23" s="351"/>
-      <c r="P23" s="351"/>
-      <c r="Q23" s="351"/>
-      <c r="R23" s="351"/>
-      <c r="S23" s="352"/>
-    </row>
-    <row r="24" spans="2:19" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="354"/>
+        <v>333</v>
+      </c>
+      <c r="K23" s="375" t="s">
+        <v>349</v>
+      </c>
+      <c r="L23" s="377"/>
+      <c r="M23" s="375"/>
+      <c r="N23" s="376"/>
+      <c r="O23" s="376"/>
+      <c r="P23" s="376"/>
+      <c r="Q23" s="376"/>
+      <c r="R23" s="376"/>
+      <c r="S23" s="377"/>
+    </row>
+    <row r="24" spans="2:19" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="379"/>
       <c r="C24" s="140"/>
       <c r="D24" s="139"/>
-      <c r="E24" s="350" t="s">
-        <v>354</v>
-      </c>
-      <c r="F24" s="351"/>
-      <c r="G24" s="351"/>
-      <c r="H24" s="352"/>
-      <c r="I24" s="350" t="s">
-        <v>294</v>
-      </c>
-      <c r="J24" s="351"/>
-      <c r="K24" s="352"/>
+      <c r="E24" s="375" t="s">
+        <v>352</v>
+      </c>
+      <c r="F24" s="376"/>
+      <c r="G24" s="376"/>
+      <c r="H24" s="377"/>
+      <c r="I24" s="375" t="s">
+        <v>293</v>
+      </c>
+      <c r="J24" s="376"/>
+      <c r="K24" s="377"/>
       <c r="L24" s="290"/>
-      <c r="M24" s="350"/>
-      <c r="N24" s="351"/>
-      <c r="O24" s="351"/>
-      <c r="P24" s="351"/>
-      <c r="Q24" s="351"/>
-      <c r="R24" s="351"/>
-      <c r="S24" s="352"/>
-    </row>
-    <row r="25" spans="2:19" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M24" s="375"/>
+      <c r="N24" s="376"/>
+      <c r="O24" s="376"/>
+      <c r="P24" s="376"/>
+      <c r="Q24" s="376"/>
+      <c r="R24" s="376"/>
+      <c r="S24" s="377"/>
+    </row>
+    <row r="25" spans="2:19" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="319" t="s">
         <v>201</v>
       </c>
@@ -7059,23 +7082,23 @@
       </c>
       <c r="E25" s="141"/>
       <c r="F25" s="141"/>
-      <c r="G25" s="360" t="s">
+      <c r="G25" s="385" t="s">
         <v>228</v>
       </c>
-      <c r="H25" s="361"/>
-      <c r="I25" s="361"/>
-      <c r="J25" s="361"/>
-      <c r="K25" s="361"/>
-      <c r="L25" s="361"/>
-      <c r="M25" s="361"/>
-      <c r="N25" s="361"/>
-      <c r="O25" s="361"/>
-      <c r="P25" s="361"/>
-      <c r="Q25" s="361"/>
-      <c r="R25" s="361"/>
-      <c r="S25" s="362"/>
-    </row>
-    <row r="26" spans="2:19" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H25" s="386"/>
+      <c r="I25" s="386"/>
+      <c r="J25" s="386"/>
+      <c r="K25" s="386"/>
+      <c r="L25" s="386"/>
+      <c r="M25" s="386"/>
+      <c r="N25" s="386"/>
+      <c r="O25" s="386"/>
+      <c r="P25" s="386"/>
+      <c r="Q25" s="386"/>
+      <c r="R25" s="386"/>
+      <c r="S25" s="387"/>
+    </row>
+    <row r="26" spans="2:19" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="320"/>
       <c r="C26" s="142"/>
       <c r="D26" s="144"/>
@@ -7088,17 +7111,17 @@
       <c r="K26" s="294"/>
       <c r="L26" s="141"/>
       <c r="M26" s="141"/>
-      <c r="N26" s="366" t="s">
+      <c r="N26" s="391" t="s">
         <v>225</v>
       </c>
-      <c r="O26" s="367"/>
-      <c r="P26" s="367"/>
-      <c r="Q26" s="367"/>
-      <c r="R26" s="367"/>
-      <c r="S26" s="368"/>
-    </row>
-    <row r="27" spans="2:19" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="357" t="s">
+      <c r="O26" s="392"/>
+      <c r="P26" s="392"/>
+      <c r="Q26" s="392"/>
+      <c r="R26" s="392"/>
+      <c r="S26" s="393"/>
+    </row>
+    <row r="27" spans="2:19" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="382" t="s">
         <v>202</v>
       </c>
       <c r="C27" s="146"/>
@@ -7108,33 +7131,33 @@
         <v>76</v>
       </c>
       <c r="G27" s="102" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H27" s="108" t="s">
         <v>229</v>
       </c>
       <c r="I27" s="105"/>
       <c r="J27" s="105" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="K27" s="108" t="s">
         <v>232</v>
       </c>
-      <c r="L27" s="355" t="s">
+      <c r="L27" s="380" t="s">
         <v>233</v>
       </c>
-      <c r="M27" s="356"/>
-      <c r="N27" s="363"/>
-      <c r="O27" s="355" t="s">
+      <c r="M27" s="381"/>
+      <c r="N27" s="388"/>
+      <c r="O27" s="380" t="s">
         <v>235</v>
       </c>
-      <c r="P27" s="356"/>
-      <c r="Q27" s="356"/>
-      <c r="R27" s="356"/>
-      <c r="S27" s="363"/>
-    </row>
-    <row r="28" spans="2:19" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="358"/>
+      <c r="P27" s="381"/>
+      <c r="Q27" s="381"/>
+      <c r="R27" s="381"/>
+      <c r="S27" s="388"/>
+    </row>
+    <row r="28" spans="2:19" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="383"/>
       <c r="C28" s="147"/>
       <c r="D28" s="147"/>
       <c r="E28" s="106"/>
@@ -7150,21 +7173,21 @@
         <v>95</v>
       </c>
       <c r="K28" s="108" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L28" s="104"/>
-      <c r="M28" s="355" t="s">
-        <v>327</v>
-      </c>
-      <c r="N28" s="356"/>
-      <c r="O28" s="369"/>
+      <c r="M28" s="380" t="s">
+        <v>325</v>
+      </c>
+      <c r="N28" s="381"/>
+      <c r="O28" s="394"/>
       <c r="P28" s="107"/>
       <c r="Q28" s="107"/>
       <c r="R28" s="107"/>
       <c r="S28" s="107"/>
     </row>
-    <row r="29" spans="2:19" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="358"/>
+    <row r="29" spans="2:19" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="383"/>
       <c r="C29" s="147"/>
       <c r="D29" s="147"/>
       <c r="E29" s="111"/>
@@ -7173,22 +7196,22 @@
       <c r="H29" s="107"/>
       <c r="I29" s="108"/>
       <c r="J29" s="108" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="K29" s="109"/>
       <c r="L29" s="295"/>
-      <c r="M29" s="364" t="s">
-        <v>363</v>
-      </c>
-      <c r="N29" s="365"/>
+      <c r="M29" s="389" t="s">
+        <v>361</v>
+      </c>
+      <c r="N29" s="390"/>
       <c r="O29" s="107"/>
       <c r="P29" s="107"/>
       <c r="Q29" s="107"/>
       <c r="R29" s="107"/>
       <c r="S29" s="107"/>
     </row>
-    <row r="30" spans="2:19" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="358"/>
+    <row r="30" spans="2:19" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="383"/>
       <c r="C30" s="147"/>
       <c r="D30" s="147"/>
       <c r="E30" s="111"/>
@@ -7196,23 +7219,23 @@
       <c r="G30" s="296"/>
       <c r="H30" s="107"/>
       <c r="I30" s="107"/>
-      <c r="J30" s="355" t="s">
-        <v>325</v>
-      </c>
-      <c r="K30" s="356"/>
+      <c r="J30" s="380" t="s">
+        <v>323</v>
+      </c>
+      <c r="K30" s="381"/>
       <c r="L30" s="108"/>
       <c r="M30" s="105"/>
-      <c r="N30" s="355" t="s">
-        <v>320</v>
-      </c>
-      <c r="O30" s="356"/>
-      <c r="P30" s="356"/>
-      <c r="Q30" s="356"/>
-      <c r="R30" s="356"/>
-      <c r="S30" s="363"/>
-    </row>
-    <row r="31" spans="2:19" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="359"/>
+      <c r="N30" s="380" t="s">
+        <v>318</v>
+      </c>
+      <c r="O30" s="381"/>
+      <c r="P30" s="381"/>
+      <c r="Q30" s="381"/>
+      <c r="R30" s="381"/>
+      <c r="S30" s="388"/>
+    </row>
+    <row r="31" spans="2:19" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="384"/>
       <c r="C31" s="148"/>
       <c r="D31" s="148"/>
       <c r="E31" s="112"/>
@@ -7231,13 +7254,13 @@
       <c r="R31" s="103"/>
       <c r="S31" s="293"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -7246,19 +7269,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="B5:S5"/>
-    <mergeCell ref="N6:S6"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="N7:S7"/>
-    <mergeCell ref="M7:M8"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="J30:K30"/>
@@ -7274,6 +7284,19 @@
     <mergeCell ref="M23:S23"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="M24:S24"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="B5:S5"/>
+    <mergeCell ref="N6:S6"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="L21">
     <cfRule type="expression" dxfId="27" priority="84">
@@ -7534,36 +7557,36 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.90625" style="42" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" style="79" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" style="42" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="79" customWidth="1"/>
     <col min="3" max="3" width="31" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" style="73" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="73" customWidth="1"/>
     <col min="5" max="5" width="31" style="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.54296875" style="44" customWidth="1"/>
+    <col min="6" max="6" width="48.5546875" style="44" customWidth="1"/>
     <col min="7" max="7" width="51" style="44" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="42" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="42" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="84"/>
       <c r="C1" s="84"/>
       <c r="D1" s="85"/>
       <c r="E1" s="86"/>
       <c r="F1" s="87"/>
     </row>
-    <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="394" t="s">
+    <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="396" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="395"/>
-      <c r="D2" s="395"/>
-      <c r="E2" s="395"/>
-      <c r="F2" s="395"/>
-      <c r="G2" s="396"/>
-    </row>
-    <row r="3" spans="1:7" s="88" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="397"/>
+      <c r="D2" s="397"/>
+      <c r="E2" s="397"/>
+      <c r="F2" s="397"/>
+      <c r="G2" s="398"/>
+    </row>
+    <row r="3" spans="1:7" s="88" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="207" t="s">
         <v>10</v>
       </c>
@@ -7571,7 +7594,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="209" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E3" s="208" t="s">
         <v>3</v>
@@ -7583,7 +7606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="213" t="s">
         <v>102</v>
       </c>
@@ -7598,7 +7621,7 @@
       <c r="F4" s="55"/>
       <c r="G4" s="328"/>
     </row>
-    <row r="5" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="221" t="s">
         <v>103</v>
       </c>
@@ -7611,11 +7634,11 @@
         <v>143</v>
       </c>
       <c r="F5" s="57" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G5" s="153"/>
     </row>
-    <row r="6" spans="1:7" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="222" t="s">
         <v>105</v>
       </c>
@@ -7628,18 +7651,18 @@
         <v>204</v>
       </c>
       <c r="F6" s="45" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G6" s="329"/>
     </row>
-    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="223"/>
       <c r="C7" s="76"/>
       <c r="D7" s="72"/>
       <c r="E7" s="80"/>
       <c r="G7" s="46"/>
     </row>
-    <row r="8" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="224" t="s">
         <v>106</v>
       </c>
@@ -7654,7 +7677,7 @@
       <c r="F8" s="55"/>
       <c r="G8" s="328"/>
     </row>
-    <row r="9" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="221" t="s">
         <v>107</v>
       </c>
@@ -7673,7 +7696,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="225" t="s">
         <v>108</v>
       </c>
@@ -7683,14 +7706,14 @@
       </c>
       <c r="D10" s="77"/>
       <c r="E10" s="80" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="F10" s="44" t="s">
-        <v>253</v>
-      </c>
       <c r="G10" s="331"/>
     </row>
-    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="71"/>
       <c r="B11" s="222" t="s">
         <v>109</v>
@@ -7701,79 +7724,79 @@
       </c>
       <c r="D11" s="90"/>
       <c r="E11" s="82" t="s">
+        <v>253</v>
+      </c>
+      <c r="F11" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="F11" s="45" t="s">
-        <v>255</v>
-      </c>
       <c r="G11" s="329"/>
     </row>
-    <row r="12" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12" s="226"/>
       <c r="D12" s="81"/>
       <c r="E12" s="80"/>
       <c r="G12" s="46"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="78"/>
       <c r="E13" s="80"/>
       <c r="G13" s="46"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="78"/>
       <c r="E14" s="80"/>
       <c r="G14" s="46"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="71"/>
       <c r="C15" s="78"/>
       <c r="E15" s="80"/>
       <c r="G15" s="46"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="78"/>
       <c r="E16" s="80"/>
       <c r="G16" s="46"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="71"/>
       <c r="C17" s="78"/>
       <c r="E17" s="80"/>
       <c r="G17" s="46"/>
     </row>
-    <row r="18" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C18" s="78"/>
-      <c r="D18" s="393"/>
+      <c r="D18" s="395"/>
       <c r="E18" s="80"/>
       <c r="G18" s="46"/>
     </row>
-    <row r="19" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C19" s="78"/>
-      <c r="D19" s="393"/>
+      <c r="D19" s="395"/>
       <c r="E19" s="80"/>
       <c r="G19" s="46"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C20" s="78"/>
       <c r="G20" s="46"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C21" s="78"/>
       <c r="G21" s="46"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C22" s="78"/>
       <c r="G22" s="46"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C23" s="78"/>
       <c r="G23" s="46"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C24" s="78"/>
       <c r="G24" s="46"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C25" s="78"/>
     </row>
   </sheetData>
@@ -7925,30 +7948,30 @@
       <selection activeCell="F17" sqref="F17:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.90625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" style="21" customWidth="1"/>
     <col min="2" max="2" width="9" style="32"/>
-    <col min="3" max="3" width="20.453125" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="39.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.453125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="44.36328125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="30" customWidth="1"/>
+    <col min="5" max="5" width="39.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.44140625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="44.33203125" style="21" customWidth="1"/>
     <col min="8" max="16384" width="9" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="399" t="s">
+    <row r="1" spans="1:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="409" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="400"/>
-      <c r="D2" s="400"/>
-      <c r="E2" s="400"/>
-      <c r="F2" s="400"/>
-      <c r="G2" s="401"/>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="410"/>
+      <c r="D2" s="410"/>
+      <c r="E2" s="410"/>
+      <c r="F2" s="410"/>
+      <c r="G2" s="411"/>
+    </row>
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="240" t="s">
         <v>10</v>
       </c>
@@ -7956,7 +7979,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="242" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E3" s="243" t="s">
         <v>3</v>
@@ -7968,7 +7991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="85.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="85.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="215" t="s">
         <v>90</v>
       </c>
@@ -7978,11 +8001,11 @@
       <c r="D4" s="48"/>
       <c r="E4" s="49"/>
       <c r="F4" s="196" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G4" s="321"/>
     </row>
-    <row r="5" spans="1:7" ht="143" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="179.4" x14ac:dyDescent="0.3">
       <c r="B5" s="267" t="s">
         <v>77</v>
       </c>
@@ -7995,11 +8018,11 @@
         <v>206</v>
       </c>
       <c r="F5" s="194" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G5" s="322"/>
     </row>
-    <row r="6" spans="1:7" ht="117" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="B6" s="267" t="s">
         <v>78</v>
       </c>
@@ -8009,85 +8032,85 @@
       </c>
       <c r="D6" s="190"/>
       <c r="E6" s="195" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F6" s="194" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G6" s="323" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="398" t="s">
+    <row r="7" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="403" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="397">
+      <c r="C7" s="402">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D7" s="402"/>
-      <c r="E7" s="404" t="s">
-        <v>342</v>
-      </c>
-      <c r="F7" s="403" t="s">
-        <v>260</v>
+      <c r="D7" s="401"/>
+      <c r="E7" s="400" t="s">
+        <v>340</v>
+      </c>
+      <c r="F7" s="399" t="s">
+        <v>259</v>
       </c>
       <c r="G7" s="323" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="398"/>
-      <c r="C8" s="397"/>
-      <c r="D8" s="402"/>
-      <c r="E8" s="404"/>
-      <c r="F8" s="403"/>
+    <row r="8" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="403"/>
+      <c r="C8" s="402"/>
+      <c r="D8" s="401"/>
+      <c r="E8" s="400"/>
+      <c r="F8" s="399"/>
       <c r="G8" s="323" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="28" customFormat="1" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="28" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31"/>
-      <c r="B9" s="398"/>
-      <c r="C9" s="397"/>
-      <c r="D9" s="402"/>
-      <c r="E9" s="404"/>
-      <c r="F9" s="403"/>
+      <c r="B9" s="403"/>
+      <c r="C9" s="402"/>
+      <c r="D9" s="401"/>
+      <c r="E9" s="400"/>
+      <c r="F9" s="399"/>
       <c r="G9" s="323" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="169.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="398" t="s">
+    <row r="10" spans="1:7" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="403" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="397">
+      <c r="C10" s="402">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D10" s="402"/>
-      <c r="E10" s="404" t="s">
+      <c r="D10" s="401"/>
+      <c r="E10" s="400" t="s">
         <v>147</v>
       </c>
-      <c r="F10" s="403" t="s">
-        <v>365</v>
+      <c r="F10" s="399" t="s">
+        <v>363</v>
       </c>
       <c r="G10" s="324" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="169.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="398"/>
-      <c r="C11" s="397"/>
-      <c r="D11" s="402"/>
-      <c r="E11" s="404"/>
-      <c r="F11" s="403"/>
+    <row r="11" spans="1:7" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="403"/>
+      <c r="C11" s="402"/>
+      <c r="D11" s="401"/>
+      <c r="E11" s="400"/>
+      <c r="F11" s="399"/>
       <c r="G11" s="324" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="218" t="s">
         <v>81</v>
       </c>
@@ -8100,19 +8123,19 @@
         <v>124</v>
       </c>
       <c r="F12" s="183" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G12" s="325" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="219"/>
       <c r="E13" s="25"/>
       <c r="F13" s="12"/>
       <c r="G13" s="22"/>
     </row>
-    <row r="14" spans="1:7" ht="55.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="220" t="s">
         <v>83</v>
       </c>
@@ -8125,11 +8148,11 @@
       </c>
       <c r="E14" s="50"/>
       <c r="F14" s="196" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G14" s="321"/>
     </row>
-    <row r="15" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="217" t="s">
         <v>82</v>
       </c>
@@ -8139,7 +8162,7 @@
       </c>
       <c r="D15" s="182"/>
       <c r="E15" s="68" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F15" s="247" t="s">
         <v>6</v>
@@ -8148,7 +8171,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="216" t="s">
         <v>148</v>
       </c>
@@ -8161,54 +8184,54 @@
         <v>152</v>
       </c>
       <c r="F16" s="192" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G16" s="326" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="398" t="s">
+    <row r="17" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="403" t="s">
         <v>149</v>
       </c>
-      <c r="C17" s="397">
+      <c r="C17" s="402">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="D17" s="402"/>
-      <c r="E17" s="404" t="s">
+      <c r="D17" s="401"/>
+      <c r="E17" s="400" t="s">
         <v>209</v>
       </c>
-      <c r="F17" s="403" t="s">
-        <v>366</v>
+      <c r="F17" s="399" t="s">
+        <v>364</v>
       </c>
       <c r="G17" s="326" t="s">
         <v>154</v>
       </c>
       <c r="K17" s="200"/>
     </row>
-    <row r="18" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="398"/>
-      <c r="C18" s="397"/>
-      <c r="D18" s="402"/>
-      <c r="E18" s="404"/>
-      <c r="F18" s="403"/>
+    <row r="18" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="403"/>
+      <c r="C18" s="402"/>
+      <c r="D18" s="401"/>
+      <c r="E18" s="400"/>
+      <c r="F18" s="399"/>
       <c r="G18" s="326" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="410"/>
-      <c r="C19" s="409"/>
-      <c r="D19" s="408"/>
-      <c r="E19" s="407"/>
-      <c r="F19" s="406"/>
+    <row r="19" spans="1:11" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="408"/>
+      <c r="C19" s="407"/>
+      <c r="D19" s="406"/>
+      <c r="E19" s="405"/>
+      <c r="F19" s="404"/>
       <c r="G19" s="327" t="s">
         <v>156</v>
       </c>
       <c r="K19" s="200"/>
     </row>
-    <row r="20" spans="1:11" s="28" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" s="28" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="31"/>
       <c r="B20" s="219"/>
       <c r="C20" s="35"/>
@@ -8217,7 +8240,7 @@
       <c r="F20" s="12"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="249" t="s">
         <v>84</v>
       </c>
@@ -8232,7 +8255,7 @@
       <c r="F21" s="181"/>
       <c r="G21" s="69"/>
     </row>
-    <row r="22" spans="1:11" ht="91" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="96.6" x14ac:dyDescent="0.3">
       <c r="B22" s="217" t="s">
         <v>86</v>
       </c>
@@ -8242,16 +8265,16 @@
       </c>
       <c r="D22" s="182"/>
       <c r="E22" s="180" t="s">
+        <v>262</v>
+      </c>
+      <c r="F22" s="181" t="s">
         <v>263</v>
-      </c>
-      <c r="F22" s="181" t="s">
-        <v>264</v>
       </c>
       <c r="G22" s="69" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="31"/>
       <c r="B23" s="280" t="s">
         <v>85</v>
@@ -8265,79 +8288,79 @@
         <v>9</v>
       </c>
       <c r="F23" s="273" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G23" s="184"/>
     </row>
-    <row r="24" spans="1:11" s="31" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="398" t="s">
+    <row r="24" spans="1:11" s="31" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="403" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="397">
+      <c r="C24" s="402">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="D24" s="402"/>
-      <c r="E24" s="405" t="s">
+      <c r="D24" s="401"/>
+      <c r="E24" s="412" t="s">
         <v>157</v>
       </c>
-      <c r="F24" s="403" t="s">
-        <v>266</v>
+      <c r="F24" s="399" t="s">
+        <v>265</v>
       </c>
       <c r="G24" s="184" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="31" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="398"/>
-      <c r="C25" s="397"/>
-      <c r="D25" s="402"/>
-      <c r="E25" s="405"/>
-      <c r="F25" s="403"/>
+    <row r="25" spans="1:11" s="31" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="403"/>
+      <c r="C25" s="402"/>
+      <c r="D25" s="401"/>
+      <c r="E25" s="412"/>
+      <c r="F25" s="399"/>
       <c r="G25" s="184" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="31" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="398"/>
-      <c r="C26" s="397"/>
-      <c r="D26" s="402"/>
-      <c r="E26" s="405"/>
-      <c r="F26" s="403"/>
+    <row r="26" spans="1:11" s="31" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="403"/>
+      <c r="C26" s="402"/>
+      <c r="D26" s="401"/>
+      <c r="E26" s="412"/>
+      <c r="F26" s="399"/>
       <c r="G26" s="184" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="31" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="398" t="s">
+    <row r="27" spans="1:11" s="31" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="403" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="397">
+      <c r="C27" s="402">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="D27" s="402"/>
-      <c r="E27" s="404" t="s">
+      <c r="D27" s="401"/>
+      <c r="E27" s="400" t="s">
         <v>133</v>
       </c>
-      <c r="F27" s="403" t="s">
-        <v>267</v>
+      <c r="F27" s="399" t="s">
+        <v>266</v>
       </c>
       <c r="G27" s="326" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="31" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="398"/>
-      <c r="C28" s="397"/>
-      <c r="D28" s="402"/>
-      <c r="E28" s="404"/>
-      <c r="F28" s="403"/>
+    <row r="28" spans="1:11" s="31" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="403"/>
+      <c r="C28" s="402"/>
+      <c r="D28" s="401"/>
+      <c r="E28" s="400"/>
+      <c r="F28" s="399"/>
       <c r="G28" s="326" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="280" t="s">
         <v>158</v>
       </c>
@@ -8350,13 +8373,13 @@
         <v>215</v>
       </c>
       <c r="F29" s="284" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G29" s="326" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="281" t="s">
         <v>159</v>
       </c>
@@ -8369,19 +8392,19 @@
         <v>7</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G30" s="38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="219"/>
       <c r="E31" s="26"/>
       <c r="F31" s="3"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="220" t="s">
         <v>88</v>
       </c>
@@ -8394,11 +8417,11 @@
       </c>
       <c r="E32" s="52"/>
       <c r="F32" s="197" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G32" s="51"/>
     </row>
-    <row r="33" spans="2:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="218" t="s">
         <v>89</v>
       </c>
@@ -8411,341 +8434,331 @@
         <v>12</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G33" s="332"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="219"/>
       <c r="E34" s="24"/>
       <c r="G34" s="22"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="219"/>
       <c r="E35" s="21"/>
       <c r="G35" s="22"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="219"/>
       <c r="E36" s="21"/>
       <c r="G36" s="22"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="219"/>
       <c r="E37" s="21"/>
       <c r="G37" s="22"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="219"/>
       <c r="E38" s="21"/>
       <c r="G38" s="22"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E39" s="21"/>
       <c r="G39" s="22"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E40" s="21"/>
       <c r="G40" s="22"/>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E41" s="21"/>
       <c r="G41" s="22"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E42" s="21"/>
       <c r="G42" s="22"/>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E43" s="21"/>
       <c r="G43" s="22"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E44" s="21"/>
       <c r="G44" s="22"/>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E45" s="21"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E47" s="21"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E48" s="21"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="21"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="21"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="21"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="21"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="21"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="21"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="22"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="22"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="22"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="22"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="22"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="22"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="22"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="22"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="22"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="22"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="22"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="22"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="22"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="22"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="22"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="22"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="22"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="22"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73" s="22"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74" s="22"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75" s="22"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76" s="22"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77" s="22"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78" s="22"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79" s="22"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80" s="22"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="22"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82" s="22"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83" s="22"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84" s="22"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85" s="22"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86" s="22"/>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E87" s="22"/>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E88" s="22"/>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E89" s="22"/>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E90" s="22"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E91" s="22"/>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E92" s="22"/>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E93" s="22"/>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E94" s="22"/>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E95" s="22"/>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E96" s="22"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97" s="22"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98" s="22"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99" s="22"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100" s="22"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101" s="22"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102" s="22"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E103" s="22"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E104" s="22"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E105" s="22"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E106" s="22"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E107" s="22"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E108" s="22"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E109" s="22"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E110" s="22"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E111" s="22"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E112" s="22"/>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E113" s="22"/>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E114" s="22"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E115" s="22"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E116" s="22"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E117" s="22"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E118" s="22"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E119" s="22"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E120" s="22"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E121" s="22"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E122" s="22"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E123" s="22"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E124" s="22"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E125" s="22"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E126" s="22"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E127" s="22"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E128" s="22"/>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E129" s="22"/>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E130" s="22"/>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E131" s="22"/>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E132" s="22"/>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E133" s="22"/>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E134" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B19"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="B2:G2"/>
@@ -8762,6 +8775,16 @@
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B27:B28"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Validation Error" error="Please select appropriate status from the list." promptTitle="Task Status" prompt="Please select the status of this task from the list." sqref="D15:D17 D33 D22:D25 D5:D7 D10:D12 D27 D29:D30" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -8983,35 +9006,35 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.90625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" style="21" customWidth="1"/>
     <col min="2" max="2" width="9" style="33"/>
-    <col min="3" max="3" width="25.453125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" style="65" customWidth="1"/>
-    <col min="5" max="5" width="39.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.36328125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="45.453125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="65" customWidth="1"/>
+    <col min="5" max="5" width="39.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.33203125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="45.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="32"/>
       <c r="C1" s="35"/>
       <c r="D1" s="30"/>
       <c r="E1" s="20"/>
     </row>
-    <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="399" t="s">
+    <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="409" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="400"/>
-      <c r="D2" s="400"/>
-      <c r="E2" s="400"/>
-      <c r="F2" s="400"/>
-      <c r="G2" s="401"/>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="410"/>
+      <c r="D2" s="410"/>
+      <c r="E2" s="410"/>
+      <c r="F2" s="410"/>
+      <c r="G2" s="411"/>
+    </row>
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="207" t="s">
         <v>10</v>
       </c>
@@ -9019,7 +9042,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="209" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E3" s="208" t="s">
         <v>3</v>
@@ -9031,7 +9054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="249" t="s">
         <v>43</v>
       </c>
@@ -9046,7 +9069,7 @@
       <c r="F4" s="181"/>
       <c r="G4" s="251"/>
     </row>
-    <row r="5" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="217" t="s">
         <v>44</v>
       </c>
@@ -9056,16 +9079,16 @@
       </c>
       <c r="D5" s="202"/>
       <c r="E5" s="341" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F5" s="193" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G5" s="201" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="31" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="31" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="21"/>
       <c r="B6" s="280" t="s">
         <v>163</v>
@@ -9076,16 +9099,16 @@
       </c>
       <c r="D6" s="285"/>
       <c r="E6" s="282" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F6" s="273" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G6" s="252" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="31" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="31" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21"/>
       <c r="B7" s="280" t="s">
         <v>165</v>
@@ -9099,53 +9122,53 @@
         <v>164</v>
       </c>
       <c r="F7" s="273" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G7" s="248" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31"/>
-      <c r="B8" s="398" t="s">
+      <c r="B8" s="403" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="397">
+      <c r="C8" s="402">
         <f t="shared" ref="C8:C17" si="0">IF(D8="Yes",0,IF(D8="No",2,IF(D8="Not Applicable","",1)))</f>
         <v>1</v>
       </c>
-      <c r="D8" s="415"/>
-      <c r="E8" s="413" t="s">
-        <v>279</v>
-      </c>
-      <c r="F8" s="412" t="s">
-        <v>281</v>
+      <c r="D8" s="417"/>
+      <c r="E8" s="415" t="s">
+        <v>278</v>
+      </c>
+      <c r="F8" s="414" t="s">
+        <v>280</v>
       </c>
       <c r="G8" s="283" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="31" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="398"/>
-      <c r="C9" s="397"/>
-      <c r="D9" s="415"/>
-      <c r="E9" s="414"/>
-      <c r="F9" s="412"/>
+    <row r="9" spans="1:7" s="31" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="403"/>
+      <c r="C9" s="402"/>
+      <c r="D9" s="417"/>
+      <c r="E9" s="416"/>
+      <c r="F9" s="414"/>
       <c r="G9" s="283" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="31" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="398"/>
-      <c r="C10" s="397"/>
-      <c r="D10" s="415"/>
-      <c r="E10" s="414"/>
-      <c r="F10" s="412"/>
+    <row r="10" spans="1:7" s="31" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="403"/>
+      <c r="C10" s="402"/>
+      <c r="D10" s="417"/>
+      <c r="E10" s="416"/>
+      <c r="F10" s="414"/>
       <c r="G10" s="283" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="280" t="s">
         <v>169</v>
       </c>
@@ -9164,7 +9187,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="31" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="31" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
       <c r="B12" s="280" t="s">
         <v>170</v>
@@ -9175,16 +9198,16 @@
       </c>
       <c r="D12" s="285"/>
       <c r="E12" s="342" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F12" s="273" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G12" s="283" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="117" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
       <c r="B13" s="280" t="s">
         <v>171</v>
       </c>
@@ -9194,16 +9217,16 @@
       </c>
       <c r="D13" s="285"/>
       <c r="E13" s="344" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G13" s="283" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="280" t="s">
         <v>172</v>
       </c>
@@ -9222,7 +9245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="280" t="s">
         <v>173</v>
@@ -9233,7 +9256,7 @@
       </c>
       <c r="D15" s="285"/>
       <c r="E15" s="342" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F15" s="284" t="s">
         <v>134</v>
@@ -9242,7 +9265,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="280" t="s">
         <v>174</v>
       </c>
@@ -9252,16 +9275,16 @@
       </c>
       <c r="D16" s="285"/>
       <c r="E16" s="342" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F16" s="284" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G16" s="184" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31"/>
       <c r="B17" s="281" t="s">
         <v>175</v>
@@ -9272,268 +9295,268 @@
       </c>
       <c r="D17" s="253"/>
       <c r="E17" s="343" t="s">
+        <v>290</v>
+      </c>
+      <c r="F17" s="183" t="s">
         <v>291</v>
-      </c>
-      <c r="F17" s="183" t="s">
-        <v>292</v>
       </c>
       <c r="G17" s="333" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" s="228"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="32"/>
     </row>
-    <row r="22" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="D22" s="411"/>
-    </row>
-    <row r="23" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D22" s="413"/>
+    </row>
+    <row r="23" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B23" s="32"/>
-      <c r="D23" s="411"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D23" s="413"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="32"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="32"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="32"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="32"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="32"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="32"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="32"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" s="32"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="32"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="32"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="32"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="32"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="32"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="32"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="32"/>
       <c r="D38" s="185"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="32"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="32"/>
       <c r="E40" s="16"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="32"/>
       <c r="E41" s="16"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="32"/>
       <c r="E42" s="16"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="32"/>
       <c r="E43" s="16"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="32"/>
       <c r="E44" s="16"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="32"/>
       <c r="E45" s="16"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="32"/>
       <c r="E46" s="16"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="32"/>
       <c r="E47" s="16"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="32"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="32"/>
       <c r="E49" s="16"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="32"/>
       <c r="E50" s="16"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="32"/>
       <c r="E51" s="16"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="32"/>
       <c r="E52" s="16"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="32"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="32"/>
       <c r="E54" s="16"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="32"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="32"/>
       <c r="E56" s="16"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="32"/>
       <c r="E57" s="16"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="32"/>
       <c r="E58" s="16"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="32"/>
       <c r="E59" s="16"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="32"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="32"/>
       <c r="E61" s="16"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="32"/>
       <c r="E62" s="16"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="32"/>
       <c r="E63" s="16"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="32"/>
       <c r="E64" s="16"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="32"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="32"/>
       <c r="E66" s="16"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="32"/>
       <c r="E67" s="16"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="32"/>
       <c r="E68" s="16"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="32"/>
       <c r="E69" s="16"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="32"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="32"/>
       <c r="E71" s="16"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="32"/>
       <c r="E72" s="16"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="32"/>
       <c r="E73" s="16"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="32"/>
       <c r="E74" s="16"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" s="32"/>
       <c r="E75" s="16"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" s="32"/>
       <c r="E76" s="16"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="32"/>
       <c r="E77" s="16"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="32"/>
       <c r="E78" s="16"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79" s="32"/>
       <c r="E79" s="16"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="32"/>
       <c r="E80" s="16"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="32"/>
       <c r="E81" s="16"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" s="32"/>
       <c r="E82" s="16"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" s="32"/>
       <c r="E83" s="16"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" s="32"/>
       <c r="E84" s="16"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" s="32"/>
       <c r="E85" s="16"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" s="32"/>
       <c r="E86" s="16"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="32"/>
       <c r="E87" s="16"/>
     </row>
@@ -9697,41 +9720,41 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.90625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" style="21" customWidth="1"/>
     <col min="2" max="2" width="9" style="32"/>
-    <col min="3" max="3" width="19.90625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="65" customWidth="1"/>
-    <col min="5" max="5" width="39.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.453125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="64.453125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="30" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="65" customWidth="1"/>
+    <col min="5" max="5" width="39.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.44140625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="64.44140625" style="21" customWidth="1"/>
     <col min="8" max="9" width="9" style="21"/>
     <col min="10" max="10" width="9" style="118"/>
     <col min="11" max="16384" width="9" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" s="35"/>
       <c r="D1" s="30"/>
     </row>
-    <row r="2" spans="1:10" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="399" t="s">
+    <row r="2" spans="1:10" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="409" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="400"/>
-      <c r="D2" s="400"/>
-      <c r="E2" s="400"/>
-      <c r="F2" s="400"/>
-      <c r="G2" s="401"/>
-    </row>
-    <row r="3" spans="1:10" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="410"/>
+      <c r="D2" s="410"/>
+      <c r="E2" s="410"/>
+      <c r="F2" s="410"/>
+      <c r="G2" s="411"/>
+    </row>
+    <row r="3" spans="1:10" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="207" t="s">
         <v>10</v>
       </c>
@@ -9739,7 +9762,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="209" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E3" s="208" t="s">
         <v>3</v>
@@ -9752,7 +9775,7 @@
       </c>
       <c r="J3" s="119"/>
     </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="220" t="s">
         <v>45</v>
       </c>
@@ -9760,144 +9783,136 @@
         <v>14</v>
       </c>
       <c r="D4" s="48">
-        <f>MAX(C5:C6)</f>
+        <f>MAX(C5:C7)</f>
         <v>1</v>
       </c>
       <c r="E4" s="49"/>
       <c r="F4" s="40"/>
       <c r="G4" s="41"/>
     </row>
-    <row r="5" spans="1:10" ht="169" x14ac:dyDescent="0.35">
-      <c r="B5" s="217" t="s">
+    <row r="5" spans="1:10" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="439" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="188">
-        <f t="shared" ref="C5:C6" si="0">IF(D5="Yes",0,IF(D5="No",2,IF(D5="Not Applicable","",1)))</f>
+      <c r="C5" s="438">
+        <f t="shared" ref="C5:C7" si="0">IF(D5="Yes",0,IF(D5="No",2,IF(D5="Not Applicable","",1)))</f>
         <v>1</v>
       </c>
-      <c r="D5" s="202"/>
-      <c r="E5" s="341" t="s">
-        <v>293</v>
-      </c>
-      <c r="F5" s="193" t="s">
-        <v>295</v>
-      </c>
-      <c r="G5" s="69" t="s">
+      <c r="D5" s="437"/>
+      <c r="E5" s="436" t="s">
+        <v>292</v>
+      </c>
+      <c r="F5" s="435" t="s">
+        <v>365</v>
+      </c>
+      <c r="G5" s="350" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="218" t="s">
+    <row r="6" spans="1:10" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="403"/>
+      <c r="C6" s="402"/>
+      <c r="D6" s="417"/>
+      <c r="E6" s="415"/>
+      <c r="F6" s="414"/>
+      <c r="G6" s="351" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="76.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="349" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="187">
+      <c r="C7" s="348">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D6" s="253"/>
-      <c r="E6" s="343" t="s">
+      <c r="D7" s="253"/>
+      <c r="E7" s="343" t="s">
+        <v>294</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="G7" s="254" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="228"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="220" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="227" t="s">
+        <v>297</v>
+      </c>
+      <c r="D9" s="48">
+        <f>MAX(C10:C16)</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="54"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:10" ht="138" x14ac:dyDescent="0.3">
+      <c r="B10" s="217" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="188">
+        <f t="shared" ref="C10:C16" si="1">IF(D10="Yes",0,IF(D10="No",2,IF(D10="Not Applicable","",1)))</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="70"/>
+      <c r="E10" s="345" t="s">
+        <v>348</v>
+      </c>
+      <c r="F10" s="193" t="s">
         <v>298</v>
       </c>
-      <c r="G6" s="254" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="228"/>
-      <c r="D7" s="23"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="220" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="227" t="s">
-        <v>299</v>
-      </c>
-      <c r="D8" s="48">
-        <f>MAX(C9:C15)</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="54"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="41"/>
-    </row>
-    <row r="9" spans="1:10" ht="130" x14ac:dyDescent="0.35">
-      <c r="B9" s="217" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="188">
-        <f t="shared" ref="C9:C15" si="1">IF(D9="Yes",0,IF(D9="No",2,IF(D9="Not Applicable","",1)))</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="345" t="s">
-        <v>350</v>
-      </c>
-      <c r="F9" s="193" t="s">
-        <v>300</v>
-      </c>
-      <c r="G9" s="416" t="s">
+      <c r="G10" s="418" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="115.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="216" t="s">
+    <row r="11" spans="1:10" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="216" t="s">
         <v>50</v>
-      </c>
-      <c r="C10" s="189">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="342" t="s">
-        <v>353</v>
-      </c>
-      <c r="F10" s="194" t="s">
-        <v>301</v>
-      </c>
-      <c r="G10" s="417"/>
-    </row>
-    <row r="11" spans="1:10" ht="176.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="216" t="s">
-        <v>51</v>
       </c>
       <c r="C11" s="189">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D11" s="66"/>
-      <c r="E11" s="198" t="s">
-        <v>179</v>
+      <c r="E11" s="342" t="s">
+        <v>351</v>
       </c>
       <c r="F11" s="194" t="s">
-        <v>302</v>
-      </c>
-      <c r="G11" s="43"/>
-    </row>
-    <row r="12" spans="1:10" ht="208" x14ac:dyDescent="0.45">
+        <v>299</v>
+      </c>
+      <c r="G11" s="419"/>
+    </row>
+    <row r="12" spans="1:10" ht="176.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="216" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="189">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D12" s="66"/>
-      <c r="E12" s="152" t="s">
-        <v>15</v>
+      <c r="E12" s="198" t="s">
+        <v>179</v>
       </c>
       <c r="F12" s="194" t="s">
-        <v>303</v>
-      </c>
-      <c r="G12" s="334"/>
-    </row>
-    <row r="13" spans="1:10" ht="70.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="31"/>
+        <v>300</v>
+      </c>
+      <c r="G12" s="43"/>
+    </row>
+    <row r="13" spans="1:10" ht="220.8" x14ac:dyDescent="0.35">
       <c r="B13" s="216" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="189">
         <f t="shared" si="1"/>
@@ -9905,144 +9920,168 @@
       </c>
       <c r="D13" s="66"/>
       <c r="E13" s="152" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" s="194" t="s">
-        <v>304</v>
-      </c>
-      <c r="G13" s="36"/>
-    </row>
-    <row r="14" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+      <c r="G13" s="334"/>
+    </row>
+    <row r="14" spans="1:10" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
       <c r="B14" s="216" t="s">
-        <v>222</v>
+        <v>53</v>
       </c>
       <c r="C14" s="189">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D14" s="66"/>
-      <c r="E14" s="340" t="s">
-        <v>336</v>
+      <c r="E14" s="152" t="s">
+        <v>16</v>
       </c>
       <c r="F14" s="194" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:10" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="218" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="187">
+    <row r="15" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31"/>
+      <c r="B15" s="216" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="189">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="D15" s="255"/>
-      <c r="E15" s="206" t="s">
-        <v>352</v>
-      </c>
-      <c r="F15" s="183"/>
-      <c r="G15" s="254"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="228"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.35">
-      <c r="D17" s="117"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="115"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="340" t="s">
+        <v>334</v>
+      </c>
+      <c r="F15" s="194" t="s">
+        <v>303</v>
+      </c>
+      <c r="G15" s="36"/>
+    </row>
+    <row r="16" spans="1:10" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="218" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="187">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="255"/>
+      <c r="E16" s="206" t="s">
+        <v>350</v>
+      </c>
+      <c r="F16" s="183"/>
+      <c r="G16" s="254"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="228"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="117"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="115"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G21" s="2"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E33" s="22"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E39" s="22"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E41" s="22"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E42" s="22"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="22"/>
     </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Validation Error" error="Please select appropriate status from the list." promptTitle="Task Status" prompt="Please select the status of this task from the list." sqref="D5:D6 D9:D15" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Validation Error" error="Please select appropriate status from the list." promptTitle="Task Status" prompt="Please select the status of this task from the list." sqref="D10:D16 D5 D7" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>_Completion_Status</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
+    <hyperlink ref="G7" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
     <hyperlink ref="G5" r:id="rId2" xr:uid="{F1605408-0052-447F-B99C-268551B5CFF6}"/>
-    <hyperlink ref="G9" r:id="rId3" xr:uid="{A04FF89D-F5D0-4306-A39A-73F1D85470B2}"/>
+    <hyperlink ref="G10" r:id="rId3" xr:uid="{A04FF89D-F5D0-4306-A39A-73F1D85470B2}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{A87698AE-8C90-443A-8648-CDFE0DD20C64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -10063,7 +10102,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C16:C990 C3:C4 C7:C8</xm:sqref>
+          <xm:sqref>C17:C991 C3:C4 C8:C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="19" id="{61F52F1B-F3C7-46C2-9E92-25986D0503F7}">
@@ -10101,7 +10140,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>D8</xm:sqref>
+          <xm:sqref>D9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="14" id="{25C5F5D0-9A72-45A5-9967-F8E90B8E0F02}">
@@ -10139,7 +10178,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C6</xm:sqref>
+          <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{A47A37B5-4CFD-418C-8CD7-E897E5D36FA2}">
@@ -10158,7 +10197,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C9</xm:sqref>
+          <xm:sqref>C10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="141" id="{5A689BC8-C014-4F29-9708-77EEB70C66B4}">
@@ -10177,7 +10216,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C10:C15</xm:sqref>
+          <xm:sqref>C11:C16</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -10192,39 +10231,37 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.90625" style="155" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" style="155" customWidth="1"/>
     <col min="2" max="2" width="9" style="171"/>
-    <col min="3" max="3" width="22.90625" style="172" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="173" customWidth="1"/>
-    <col min="5" max="5" width="39.453125" style="174" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.453125" style="160" customWidth="1"/>
-    <col min="7" max="7" width="48.36328125" style="160" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" style="172" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="173" customWidth="1"/>
+    <col min="5" max="5" width="39.44140625" style="174" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.44140625" style="160" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" style="160" customWidth="1"/>
     <col min="8" max="16384" width="9" style="160"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="155" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="155" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="156"/>
       <c r="C1" s="157"/>
       <c r="D1" s="158"/>
       <c r="E1" s="159"/>
     </row>
-    <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="418" t="s">
+    <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="420" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="419"/>
-      <c r="D2" s="419"/>
-      <c r="E2" s="419"/>
-      <c r="F2" s="419"/>
-      <c r="G2" s="420"/>
-    </row>
-    <row r="3" spans="1:7" s="161" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="421"/>
+      <c r="D2" s="421"/>
+      <c r="E2" s="421"/>
+      <c r="F2" s="421"/>
+      <c r="G2" s="422"/>
+    </row>
+    <row r="3" spans="1:7" s="161" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="229" t="s">
         <v>10</v>
       </c>
@@ -10232,7 +10269,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="209" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E3" s="230" t="s">
         <v>3</v>
@@ -10244,7 +10281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="232" t="s">
         <v>55</v>
       </c>
@@ -10259,7 +10296,7 @@
       <c r="F4" s="164"/>
       <c r="G4" s="165"/>
     </row>
-    <row r="5" spans="1:7" ht="117" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
       <c r="B5" s="233" t="s">
         <v>56</v>
       </c>
@@ -10268,17 +10305,17 @@
         <v>1</v>
       </c>
       <c r="D5" s="167"/>
-      <c r="E5" s="349" t="s">
+      <c r="E5" s="347" t="s">
         <v>223</v>
       </c>
       <c r="F5" s="44" t="s">
-        <v>306</v>
-      </c>
-      <c r="G5" s="347" t="s">
+        <v>304</v>
+      </c>
+      <c r="G5" s="324" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="233" t="s">
         <v>57</v>
       </c>
@@ -10291,13 +10328,13 @@
         <v>226</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>307</v>
-      </c>
-      <c r="G6" s="347" t="s">
+        <v>305</v>
+      </c>
+      <c r="G6" s="324" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="234" t="s">
         <v>127</v>
       </c>
@@ -10310,19 +10347,17 @@
         <v>227</v>
       </c>
       <c r="F7" s="199" t="s">
-        <v>308</v>
-      </c>
-      <c r="G7" s="348" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+      <c r="G7" s="434"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G14" s="177"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="175"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="175"/>
     </row>
   </sheetData>
@@ -10334,8 +10369,12 @@
       <formula1>_Completion_Status</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{AF591578-0EE0-4AC2-A72F-B4073E678DC5}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{BD0DBFD7-DE10-4E33-ABD0-BCED2023B2D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -10451,35 +10490,35 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.90625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" style="21" customWidth="1"/>
     <col min="2" max="2" width="9" style="34"/>
-    <col min="3" max="3" width="17.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="62" customWidth="1"/>
-    <col min="5" max="5" width="39.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.453125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="50.36328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="39.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="50.33203125" style="5" customWidth="1"/>
     <col min="8" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="21" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" s="21" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="32"/>
       <c r="C1" s="35"/>
       <c r="D1" s="30"/>
       <c r="E1" s="20"/>
     </row>
-    <row r="2" spans="1:11" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="418" t="s">
+    <row r="2" spans="1:11" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="420" t="s">
         <v>191</v>
       </c>
-      <c r="C2" s="419"/>
-      <c r="D2" s="419"/>
-      <c r="E2" s="419"/>
-      <c r="F2" s="419"/>
-      <c r="G2" s="420"/>
-    </row>
-    <row r="3" spans="1:11" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="421"/>
+      <c r="D2" s="421"/>
+      <c r="E2" s="421"/>
+      <c r="F2" s="421"/>
+      <c r="G2" s="422"/>
+    </row>
+    <row r="3" spans="1:11" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="207" t="s">
         <v>10</v>
       </c>
@@ -10487,7 +10526,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="209" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E3" s="208" t="s">
         <v>3</v>
@@ -10499,7 +10538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="236" t="s">
         <v>58</v>
       </c>
@@ -10514,7 +10553,7 @@
       <c r="F4" s="57"/>
       <c r="G4" s="58"/>
     </row>
-    <row r="5" spans="1:11" s="10" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" s="10" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
       <c r="B5" s="237" t="s">
         <v>59</v>
@@ -10528,16 +10567,16 @@
         <v>135</v>
       </c>
       <c r="F5" s="204" t="s">
-        <v>310</v>
-      </c>
-      <c r="G5" s="423" t="s">
+        <v>308</v>
+      </c>
+      <c r="G5" s="425" t="s">
         <v>186</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31"/>
       <c r="B6" s="269" t="s">
         <v>60</v>
@@ -10548,14 +10587,14 @@
       </c>
       <c r="D6" s="265"/>
       <c r="E6" s="344" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>311</v>
-      </c>
-      <c r="G6" s="424"/>
-    </row>
-    <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+      <c r="G6" s="426"/>
+    </row>
+    <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31"/>
       <c r="B7" s="269" t="s">
         <v>61</v>
@@ -10568,14 +10607,14 @@
       <c r="E7" s="260" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="421" t="s">
-        <v>312</v>
-      </c>
-      <c r="G7" s="424" t="s">
+      <c r="F7" s="423" t="s">
+        <v>310</v>
+      </c>
+      <c r="G7" s="426" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31"/>
       <c r="B8" s="270" t="s">
         <v>97</v>
@@ -10586,16 +10625,16 @@
       </c>
       <c r="D8" s="271"/>
       <c r="E8" s="346" t="s">
-        <v>359</v>
-      </c>
-      <c r="F8" s="422"/>
-      <c r="G8" s="425"/>
-    </row>
-    <row r="9" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+        <v>357</v>
+      </c>
+      <c r="F8" s="424"/>
+      <c r="G8" s="427"/>
+    </row>
+    <row r="9" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="238"/>
       <c r="E9" s="22"/>
     </row>
-    <row r="10" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="239" t="s">
         <v>62</v>
       </c>
@@ -10610,7 +10649,7 @@
       <c r="F10" s="55"/>
       <c r="G10" s="56"/>
     </row>
-    <row r="11" spans="1:11" ht="65" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="69" x14ac:dyDescent="0.3">
       <c r="B11" s="237" t="s">
         <v>63</v>
       </c>
@@ -10623,11 +10662,11 @@
         <v>22</v>
       </c>
       <c r="F11" s="57" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G11" s="58"/>
     </row>
-    <row r="12" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="286" t="s">
         <v>64</v>
       </c>
@@ -10637,16 +10676,16 @@
       </c>
       <c r="D12" s="272"/>
       <c r="E12" s="344" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>314</v>
-      </c>
-      <c r="G12" s="424" t="s">
+        <v>312</v>
+      </c>
+      <c r="G12" s="426" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="286" t="s">
         <v>65</v>
       </c>
@@ -10659,11 +10698,11 @@
         <v>21</v>
       </c>
       <c r="F13" s="44" t="s">
-        <v>315</v>
-      </c>
-      <c r="G13" s="424"/>
-    </row>
-    <row r="14" spans="1:11" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>313</v>
+      </c>
+      <c r="G13" s="426"/>
+    </row>
+    <row r="14" spans="1:11" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="287" t="s">
         <v>66</v>
       </c>
@@ -10673,19 +10712,19 @@
       </c>
       <c r="D14" s="288"/>
       <c r="E14" s="346" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F14" s="45" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G14" s="47"/>
     </row>
-    <row r="15" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="238"/>
       <c r="E15" s="11"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="49.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="49.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="31"/>
       <c r="B16" s="239" t="s">
         <v>67</v>
@@ -10701,7 +10740,7 @@
       <c r="F16" s="55"/>
       <c r="G16" s="336"/>
     </row>
-    <row r="17" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="237" t="s">
         <v>68</v>
       </c>
@@ -10714,13 +10753,13 @@
         <v>20</v>
       </c>
       <c r="F17" s="57" t="s">
-        <v>317</v>
-      </c>
-      <c r="G17" s="423" t="s">
+        <v>315</v>
+      </c>
+      <c r="G17" s="425" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="233" t="s">
         <v>69</v>
@@ -10734,11 +10773,11 @@
         <v>231</v>
       </c>
       <c r="F18" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="G18" s="424"/>
-    </row>
-    <row r="19" spans="1:7" ht="52" x14ac:dyDescent="0.35">
+        <v>316</v>
+      </c>
+      <c r="G18" s="426"/>
+    </row>
+    <row r="19" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
       <c r="B19" s="233" t="s">
         <v>70</v>
       </c>
@@ -10748,14 +10787,14 @@
       </c>
       <c r="D19" s="186"/>
       <c r="E19" s="344" t="s">
+        <v>317</v>
+      </c>
+      <c r="F19" s="44" t="s">
         <v>319</v>
       </c>
-      <c r="F19" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="G19" s="424"/>
-    </row>
-    <row r="20" spans="1:7" ht="78.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G19" s="426"/>
+    </row>
+    <row r="20" spans="1:7" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="234" t="s">
         <v>71</v>
       </c>
@@ -10768,17 +10807,17 @@
         <v>136</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G20" s="337" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="238"/>
       <c r="E21" s="22"/>
     </row>
-    <row r="22" spans="1:7" s="160" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" s="160" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="175"/>
       <c r="B22" s="239" t="s">
         <v>72</v>
@@ -10794,7 +10833,7 @@
       <c r="F22" s="164"/>
       <c r="G22" s="56"/>
     </row>
-    <row r="23" spans="1:7" s="160" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" s="160" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="155"/>
       <c r="B23" s="237" t="s">
         <v>73</v>
@@ -10805,16 +10844,16 @@
       </c>
       <c r="D23" s="256"/>
       <c r="E23" s="341" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F23" s="193" t="s">
-        <v>323</v>
-      </c>
-      <c r="G23" s="423" t="s">
+        <v>321</v>
+      </c>
+      <c r="G23" s="425" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="160" customFormat="1" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" s="160" customFormat="1" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="155"/>
       <c r="B24" s="234" t="s">
         <v>74</v>
@@ -10830,13 +10869,13 @@
       <c r="F24" s="257" t="s">
         <v>190</v>
       </c>
-      <c r="G24" s="425"/>
-    </row>
-    <row r="25" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G24" s="427"/>
+    </row>
+    <row r="25" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="238"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="236" t="s">
         <v>192</v>
       </c>
@@ -10851,7 +10890,7 @@
       <c r="F26" s="57"/>
       <c r="G26" s="58"/>
     </row>
-    <row r="27" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="237" t="s">
         <v>193</v>
       </c>
@@ -10861,265 +10900,265 @@
       </c>
       <c r="D27" s="151"/>
       <c r="E27" s="345" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F27" s="57" t="s">
         <v>137</v>
       </c>
       <c r="G27" s="58"/>
     </row>
-    <row r="28" spans="1:7" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="426" t="s">
+    <row r="28" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="428" t="s">
         <v>198</v>
       </c>
-      <c r="C28" s="397">
+      <c r="C28" s="402">
         <f t="shared" ref="C28" si="4">IF(D28="Yes",0,IF(D28="No",2,IF(D28="Not Applicable","",1)))</f>
         <v>1</v>
       </c>
-      <c r="D28" s="393"/>
-      <c r="E28" s="414" t="s">
+      <c r="D28" s="395"/>
+      <c r="E28" s="416" t="s">
         <v>189</v>
       </c>
-      <c r="F28" s="429" t="s">
-        <v>324</v>
+      <c r="F28" s="431" t="s">
+        <v>322</v>
       </c>
       <c r="G28" s="335" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="31.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="427"/>
-      <c r="C29" s="409"/>
-      <c r="D29" s="431"/>
-      <c r="E29" s="428"/>
-      <c r="F29" s="430"/>
+    <row r="29" spans="1:7" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="429"/>
+      <c r="C29" s="407"/>
+      <c r="D29" s="433"/>
+      <c r="E29" s="430"/>
+      <c r="F29" s="432"/>
       <c r="G29" s="338" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E39" s="22"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E41" s="22"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E42" s="22"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E48" s="9"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="9"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="9"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="9"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="9"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="9"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="9"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="9"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="9"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="9"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="9"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="9"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="9"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="9"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="9"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75" s="9"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76" s="9"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78" s="9"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79" s="9"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80" s="9"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="9"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82" s="9"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84" s="9"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85" s="9"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86" s="9"/>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E87" s="9"/>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E88" s="9"/>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E89" s="9"/>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E90" s="9"/>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E92" s="9"/>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E94" s="9"/>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E95" s="9"/>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E96" s="9"/>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97" s="9"/>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98" s="9"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99" s="9"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100" s="9"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101" s="9"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102" s="9"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E103" s="9"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E104" s="9"/>
     </row>
   </sheetData>

</xml_diff>